<commit_message>
prepare figures for manuscript
also changed a bit the GUI for graph analysis
</commit_message>
<xml_diff>
--- a/data/validation_cohort.xlsx
+++ b/data/validation_cohort.xlsx
@@ -716,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z2" workbookViewId="0">
-      <selection activeCell="AJ30" sqref="AJ30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>